<commit_message>
Vladimir ir Toma vienodai
</commit_message>
<xml_diff>
--- a/Dienynas JAVA 1007.xlsx
+++ b/Dienynas JAVA 1007.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="187">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -496,6 +496,93 @@
   </si>
   <si>
     <t>01 16</t>
+  </si>
+  <si>
+    <t>01 17</t>
+  </si>
+  <si>
+    <t>01 20</t>
+  </si>
+  <si>
+    <t>01 22</t>
+  </si>
+  <si>
+    <t>01 21</t>
+  </si>
+  <si>
+    <t>01 23</t>
+  </si>
+  <si>
+    <t>01 24</t>
+  </si>
+  <si>
+    <t>01 27</t>
+  </si>
+  <si>
+    <t>01 28</t>
+  </si>
+  <si>
+    <t>01 29</t>
+  </si>
+  <si>
+    <t>01 30</t>
+  </si>
+  <si>
+    <t>01 31</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>02 03</t>
+  </si>
+  <si>
+    <t>02 04</t>
+  </si>
+  <si>
+    <t>02 05</t>
+  </si>
+  <si>
+    <t>02 06</t>
+  </si>
+  <si>
+    <t>02 07</t>
+  </si>
+  <si>
+    <t>02 10</t>
+  </si>
+  <si>
+    <t>02 11</t>
+  </si>
+  <si>
+    <t>02 12</t>
+  </si>
+  <si>
+    <t>02 13</t>
+  </si>
+  <si>
+    <t>02 14</t>
+  </si>
+  <si>
+    <t>02 17</t>
+  </si>
+  <si>
+    <t>02 18</t>
+  </si>
+  <si>
+    <t>02 19</t>
+  </si>
+  <si>
+    <t>02 20</t>
+  </si>
+  <si>
+    <t>02 21</t>
   </si>
 </sst>
 </file>
@@ -705,7 +792,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -793,24 +880,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -838,6 +907,30 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1143,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
@@ -1230,49 +1323,49 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="39" t="s">
         <v>103</v>
       </c>
       <c r="P3" s="14"/>
@@ -1287,62 +1380,62 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="37" t="s">
+      <c r="AB3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="39" t="s">
         <v>115</v>
       </c>
       <c r="P4" s="14"/>
@@ -1357,11 +1450,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
@@ -1370,43 +1463,43 @@
       <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="N5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="O5" s="43" t="s">
+      <c r="C5" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="37" t="s">
         <v>100</v>
       </c>
       <c r="P5" s="10"/>
@@ -1420,7 +1513,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="39" t="s">
+      <c r="AB5" s="33" t="s">
         <v>78</v>
       </c>
       <c r="AC5" s="10">
@@ -1461,7 +1554,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="39" t="s">
+      <c r="AB6" s="33" t="s">
         <v>79</v>
       </c>
       <c r="AC6" s="10">
@@ -1502,7 +1595,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="39" t="s">
+      <c r="AB7" s="33" t="s">
         <v>79</v>
       </c>
       <c r="AC7" s="10">
@@ -1543,7 +1636,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="39" t="s">
+      <c r="AB8" s="33" t="s">
         <v>80</v>
       </c>
       <c r="AC8" s="10">
@@ -1584,7 +1677,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="39" t="s">
+      <c r="AB9" s="33" t="s">
         <v>81</v>
       </c>
       <c r="AC9" s="10">
@@ -1625,7 +1718,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="39" t="s">
+      <c r="AB10" s="33" t="s">
         <v>82</v>
       </c>
       <c r="AC10" s="10">
@@ -1666,7 +1759,7 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="39" t="s">
+      <c r="AB11" s="33" t="s">
         <v>83</v>
       </c>
       <c r="AC11" s="10">
@@ -1707,7 +1800,7 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="39" t="s">
+      <c r="AB12" s="33" t="s">
         <v>84</v>
       </c>
       <c r="AC12" s="10">
@@ -1748,7 +1841,7 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="39" t="s">
+      <c r="AB13" s="33" t="s">
         <v>85</v>
       </c>
       <c r="AC13" s="10">
@@ -1789,7 +1882,7 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="39" t="s">
+      <c r="AB14" s="33" t="s">
         <v>86</v>
       </c>
       <c r="AC14" s="10">
@@ -1830,7 +1923,7 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-      <c r="AB15" s="39" t="s">
+      <c r="AB15" s="33" t="s">
         <v>87</v>
       </c>
       <c r="AC15" s="10">
@@ -1871,7 +1964,7 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-      <c r="AB16" s="39" t="s">
+      <c r="AB16" s="33" t="s">
         <v>88</v>
       </c>
       <c r="AC16" s="10">
@@ -1912,7 +2005,7 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
-      <c r="AB17" s="39" t="s">
+      <c r="AB17" s="33" t="s">
         <v>89</v>
       </c>
       <c r="AC17" s="10">
@@ -2071,40 +2164,40 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="39" t="s">
         <v>114</v>
       </c>
       <c r="M3" s="14"/>
@@ -2122,53 +2215,53 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="37" t="s">
+      <c r="AB3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="39" t="s">
         <v>103</v>
       </c>
       <c r="M4" s="14"/>
@@ -2186,11 +2279,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="23">
@@ -2243,7 +2336,7 @@
       <c r="X5" s="17"/>
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
-      <c r="AB5" s="39" t="s">
+      <c r="AB5" s="33" t="s">
         <v>63</v>
       </c>
       <c r="AC5" s="10">
@@ -2286,7 +2379,7 @@
       <c r="X6" s="17"/>
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
-      <c r="AB6" s="39" t="s">
+      <c r="AB6" s="33" t="s">
         <v>63</v>
       </c>
       <c r="AC6" s="10">
@@ -2327,7 +2420,7 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
-      <c r="AB7" s="39" t="s">
+      <c r="AB7" s="33" t="s">
         <v>64</v>
       </c>
       <c r="AC7" s="10">
@@ -2368,7 +2461,7 @@
       <c r="X8" s="17"/>
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
-      <c r="AB8" s="39" t="s">
+      <c r="AB8" s="33" t="s">
         <v>65</v>
       </c>
       <c r="AC8" s="10">
@@ -2409,7 +2502,7 @@
       <c r="X9" s="17"/>
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
-      <c r="AB9" s="39" t="s">
+      <c r="AB9" s="33" t="s">
         <v>66</v>
       </c>
       <c r="AC9" s="10">
@@ -2450,7 +2543,7 @@
       <c r="X10" s="17"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
-      <c r="AB10" s="39" t="s">
+      <c r="AB10" s="33" t="s">
         <v>67</v>
       </c>
       <c r="AC10" s="10">
@@ -2569,7 +2662,7 @@
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
-      <c r="AB13" s="39" t="s">
+      <c r="AB13" s="33" t="s">
         <v>68</v>
       </c>
       <c r="AC13" s="10">
@@ -2610,7 +2703,7 @@
       <c r="X14" s="17"/>
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
-      <c r="AB14" s="39" t="s">
+      <c r="AB14" s="33" t="s">
         <v>69</v>
       </c>
       <c r="AC14" s="10">
@@ -2651,7 +2744,7 @@
       <c r="X15" s="17"/>
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
-      <c r="AB15" s="39" t="s">
+      <c r="AB15" s="33" t="s">
         <v>127</v>
       </c>
       <c r="AC15" s="10">
@@ -2692,7 +2785,7 @@
       <c r="X16" s="17"/>
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
-      <c r="AB16" s="39" t="s">
+      <c r="AB16" s="33" t="s">
         <v>128</v>
       </c>
       <c r="AC16" s="10">
@@ -2764,7 +2857,7 @@
   <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,24 +2943,48 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="C3" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="O3" s="14"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -2881,37 +2998,61 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -2925,11 +3066,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -2938,18 +3079,42 @@
       <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -2962,7 +3127,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="10"/>
+      <c r="AB5" s="10" t="s">
+        <v>158</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -3001,7 +3168,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="10"/>
+      <c r="AB6" s="10" t="s">
+        <v>159</v>
+      </c>
       <c r="AC6" s="10">
         <v>4</v>
       </c>
@@ -3040,7 +3209,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="10"/>
+      <c r="AB7" s="10" t="s">
+        <v>159</v>
+      </c>
       <c r="AC7" s="10">
         <v>4</v>
       </c>
@@ -3079,7 +3250,9 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="10"/>
+      <c r="AB8" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="AC8" s="10">
         <v>8</v>
       </c>
@@ -3118,7 +3291,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="10"/>
+      <c r="AB9" s="10" t="s">
+        <v>160</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -3157,7 +3332,9 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="10"/>
+      <c r="AB10" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -3196,7 +3373,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="10"/>
+      <c r="AB11" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -3235,7 +3414,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="10"/>
+      <c r="AB12" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -3274,7 +3455,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="10"/>
+      <c r="AB13" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -3313,7 +3496,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="AB14" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -3352,7 +3537,9 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-      <c r="AB15" s="10"/>
+      <c r="AB15" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="AC15" s="10">
         <v>8</v>
       </c>
@@ -3391,7 +3578,9 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-      <c r="AB16" s="10"/>
+      <c r="AB16" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="AC16" s="10">
         <v>8</v>
       </c>
@@ -3430,7 +3619,9 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
-      <c r="AB17" s="10"/>
+      <c r="AB17" s="10" t="s">
+        <v>172</v>
+      </c>
       <c r="AC17" s="10">
         <v>8</v>
       </c>
@@ -3586,64 +3777,64 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="38">
         <v>10</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="38">
         <v>10</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="38">
         <v>10</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="38">
         <v>10</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="38">
         <v>10</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="38">
         <v>11</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="38">
         <v>11</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="38">
         <v>11</v>
       </c>
-      <c r="K3" s="44">
+      <c r="K3" s="38">
         <v>11</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="38">
         <v>11</v>
       </c>
-      <c r="M3" s="44">
+      <c r="M3" s="38">
         <v>11</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="38">
         <v>11</v>
       </c>
-      <c r="O3" s="44">
+      <c r="O3" s="38">
         <v>12</v>
       </c>
-      <c r="P3" s="44">
+      <c r="P3" s="38">
         <v>12</v>
       </c>
-      <c r="Q3" s="44">
+      <c r="Q3" s="38">
         <v>12</v>
       </c>
-      <c r="R3" s="44">
+      <c r="R3" s="38">
         <v>12</v>
       </c>
-      <c r="S3" s="47" t="s">
+      <c r="S3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="T3" s="47" t="s">
+      <c r="T3" s="41" t="s">
         <v>151</v>
       </c>
       <c r="U3" s="9"/>
@@ -3653,77 +3844,77 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="44">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="38">
         <v>16</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="38">
         <v>17</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="38">
         <v>18</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="38">
         <v>21</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="38">
         <v>22</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="38">
         <v>21</v>
       </c>
-      <c r="I4" s="44">
+      <c r="I4" s="38">
         <v>22</v>
       </c>
-      <c r="J4" s="44">
+      <c r="J4" s="38">
         <v>25</v>
       </c>
-      <c r="K4" s="44">
-        <v>26</v>
-      </c>
-      <c r="L4" s="44">
+      <c r="K4" s="38">
+        <v>26</v>
+      </c>
+      <c r="L4" s="38">
         <v>27</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="38">
         <v>28</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="38">
         <v>29</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="P4" s="47" t="s">
+      <c r="P4" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="R4" s="47" t="s">
+      <c r="R4" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="S4" s="47" t="s">
+      <c r="S4" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="T4" s="44">
+      <c r="T4" s="38">
         <v>10</v>
       </c>
       <c r="U4" s="9"/>
@@ -3733,11 +3924,11 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3806,7 +3997,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="37" t="s">
         <v>95</v>
       </c>
       <c r="AC5" s="10">
@@ -3847,7 +4038,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="37" t="s">
         <v>96</v>
       </c>
       <c r="AC6" s="10">
@@ -3888,7 +4079,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="43" t="s">
+      <c r="AB7" s="37" t="s">
         <v>119</v>
       </c>
       <c r="AC7" s="10">
@@ -3929,7 +4120,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="43" t="s">
+      <c r="AB8" s="37" t="s">
         <v>152</v>
       </c>
       <c r="AC8" s="10">
@@ -3970,7 +4161,7 @@
       <c r="X9" s="30"/>
       <c r="Y9" s="30"/>
       <c r="Z9" s="30"/>
-      <c r="AB9" s="42" t="s">
+      <c r="AB9" s="36" t="s">
         <v>70</v>
       </c>
       <c r="AC9" s="30">
@@ -4012,7 +4203,7 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
-      <c r="AB10" s="43" t="s">
+      <c r="AB10" s="37" t="s">
         <v>72</v>
       </c>
       <c r="AC10" s="10">
@@ -4054,7 +4245,7 @@
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
-      <c r="AB11" s="43" t="s">
+      <c r="AB11" s="37" t="s">
         <v>120</v>
       </c>
       <c r="AC11" s="10">
@@ -4096,7 +4287,7 @@
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
       <c r="AA12" s="10"/>
-      <c r="AB12" s="43" t="s">
+      <c r="AB12" s="37" t="s">
         <v>153</v>
       </c>
       <c r="AC12" s="10">
@@ -4138,7 +4329,7 @@
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
       <c r="AA13" s="10"/>
-      <c r="AB13" s="43" t="s">
+      <c r="AB13" s="37" t="s">
         <v>73</v>
       </c>
       <c r="AC13" s="10">
@@ -4180,7 +4371,7 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
-      <c r="AB14" s="43" t="s">
+      <c r="AB14" s="37" t="s">
         <v>121</v>
       </c>
       <c r="AC14" s="10">
@@ -4222,7 +4413,7 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
-      <c r="AB15" s="43" t="s">
+      <c r="AB15" s="37" t="s">
         <v>97</v>
       </c>
       <c r="AC15" s="10">
@@ -4264,7 +4455,7 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
-      <c r="AB16" s="43" t="s">
+      <c r="AB16" s="37" t="s">
         <v>122</v>
       </c>
       <c r="AC16" s="10">
@@ -4306,7 +4497,7 @@
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
-      <c r="AB17" s="43" t="s">
+      <c r="AB17" s="37" t="s">
         <v>74</v>
       </c>
       <c r="AC17" s="10">
@@ -4348,7 +4539,7 @@
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
-      <c r="AB18" s="43" t="s">
+      <c r="AB18" s="37" t="s">
         <v>71</v>
       </c>
       <c r="AC18" s="10">
@@ -4390,7 +4581,7 @@
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
-      <c r="AB19" s="43" t="s">
+      <c r="AB19" s="37" t="s">
         <v>98</v>
       </c>
       <c r="AC19" s="10">
@@ -4432,7 +4623,7 @@
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
-      <c r="AB20" s="43" t="s">
+      <c r="AB20" s="37" t="s">
         <v>99</v>
       </c>
       <c r="AC20" s="10">
@@ -4474,7 +4665,7 @@
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
-      <c r="AB21" s="43" t="s">
+      <c r="AB21" s="37" t="s">
         <v>123</v>
       </c>
       <c r="AC21" s="10">
@@ -4516,7 +4707,7 @@
       <c r="Y22" s="10"/>
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
-      <c r="AB22" s="43" t="s">
+      <c r="AB22" s="37" t="s">
         <v>126</v>
       </c>
       <c r="AC22" s="10">
@@ -4747,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
@@ -4834,37 +5025,37 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="38">
         <v>10</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="38">
         <v>10</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="38">
         <v>10</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="38">
         <v>12</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="38">
         <v>12</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="41" t="s">
         <v>151</v>
       </c>
       <c r="L3" s="9"/>
@@ -4883,50 +5074,50 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="44">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="38">
         <v>23</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="38">
         <v>24</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="38">
         <v>25</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="47" t="s">
+      <c r="K4" s="41" t="s">
         <v>101</v>
       </c>
       <c r="L4" s="9"/>
@@ -4945,11 +5136,11 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -5000,7 +5191,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="37" t="s">
         <v>124</v>
       </c>
       <c r="AC5" s="10">
@@ -5041,7 +5232,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="37" t="s">
         <v>143</v>
       </c>
       <c r="AC6" s="10">
@@ -5082,7 +5273,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="43" t="s">
+      <c r="AB7" s="37" t="s">
         <v>76</v>
       </c>
       <c r="AC7" s="10">
@@ -5123,7 +5314,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="43" t="s">
+      <c r="AB8" s="37" t="s">
         <v>77</v>
       </c>
       <c r="AC8" s="10">
@@ -5164,7 +5355,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="43" t="s">
+      <c r="AB9" s="37" t="s">
         <v>144</v>
       </c>
       <c r="AC9" s="10">
@@ -5205,7 +5396,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="43" t="s">
+      <c r="AB10" s="37" t="s">
         <v>145</v>
       </c>
       <c r="AC10" s="10">
@@ -5285,7 +5476,7 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="43" t="s">
+      <c r="AB12" s="37" t="s">
         <v>75</v>
       </c>
       <c r="AC12" s="10">
@@ -5326,7 +5517,7 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="43" t="s">
+      <c r="AB13" s="37" t="s">
         <v>125</v>
       </c>
       <c r="AC13" s="10">
@@ -5367,7 +5558,7 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="43" t="s">
+      <c r="AB14" s="37" t="s">
         <v>146</v>
       </c>
       <c r="AC14" s="10">
@@ -5564,46 +5755,46 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="45" t="s">
+      <c r="N3" s="39" t="s">
         <v>151</v>
       </c>
       <c r="O3" s="14"/>
@@ -5619,59 +5810,59 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="39" t="s">
         <v>130</v>
       </c>
       <c r="O4" s="14"/>
@@ -5687,11 +5878,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -5700,40 +5891,40 @@
       <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="M5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="N5" s="43" t="s">
+      <c r="C5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="37" t="s">
         <v>100</v>
       </c>
       <c r="O5" s="10"/>
@@ -5748,7 +5939,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="37" t="s">
         <v>129</v>
       </c>
       <c r="AC5" s="10">
@@ -5789,7 +5980,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="37" t="s">
         <v>132</v>
       </c>
       <c r="AC6" s="10">
@@ -5830,7 +6021,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="43" t="s">
+      <c r="AB7" s="37" t="s">
         <v>133</v>
       </c>
       <c r="AC7" s="10">
@@ -5871,7 +6062,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="43" t="s">
+      <c r="AB8" s="37" t="s">
         <v>134</v>
       </c>
       <c r="AC8" s="10">
@@ -5912,7 +6103,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="43" t="s">
+      <c r="AB9" s="37" t="s">
         <v>135</v>
       </c>
       <c r="AC9" s="10">
@@ -5953,7 +6144,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="43" t="s">
+      <c r="AB10" s="37" t="s">
         <v>136</v>
       </c>
       <c r="AC10" s="10">
@@ -5994,7 +6185,7 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="43" t="s">
+      <c r="AB11" s="37" t="s">
         <v>137</v>
       </c>
       <c r="AC11" s="10">
@@ -6035,7 +6226,7 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="43" t="s">
+      <c r="AB12" s="37" t="s">
         <v>138</v>
       </c>
       <c r="AC12" s="10">
@@ -6076,7 +6267,7 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="43" t="s">
+      <c r="AB13" s="37" t="s">
         <v>139</v>
       </c>
       <c r="AC13" s="10">
@@ -6117,7 +6308,7 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="43" t="s">
+      <c r="AB14" s="37" t="s">
         <v>140</v>
       </c>
       <c r="AC14" s="10">
@@ -6158,7 +6349,7 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-      <c r="AB15" s="43" t="s">
+      <c r="AB15" s="37" t="s">
         <v>141</v>
       </c>
       <c r="AC15" s="10">
@@ -6199,7 +6390,7 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-      <c r="AB16" s="43" t="s">
+      <c r="AB16" s="37" t="s">
         <v>142</v>
       </c>
       <c r="AC16" s="10">
@@ -6270,8 +6461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6357,25 +6548,51 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="C3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
@@ -6388,38 +6605,64 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="37" t="s">
+      <c r="AB3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>118</v>
+      </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14"/>
@@ -6432,11 +6675,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -6445,19 +6688,45 @@
       <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
@@ -6469,7 +6738,9 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="17"/>
+      <c r="AB5" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="AC5" s="10">
         <v>8</v>
       </c>
@@ -6508,7 +6779,9 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="17"/>
+      <c r="AB6" s="17" t="s">
+        <v>174</v>
+      </c>
       <c r="AC6" s="10">
         <v>8</v>
       </c>
@@ -6547,7 +6820,9 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="17"/>
+      <c r="AB7" s="17" t="s">
+        <v>175</v>
+      </c>
       <c r="AC7" s="10">
         <v>8</v>
       </c>
@@ -6586,7 +6861,9 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="17"/>
+      <c r="AB8" s="17" t="s">
+        <v>176</v>
+      </c>
       <c r="AC8" s="10">
         <v>8</v>
       </c>
@@ -6625,7 +6902,9 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="17"/>
+      <c r="AB9" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="AC9" s="10">
         <v>8</v>
       </c>
@@ -6664,7 +6943,9 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="17"/>
+      <c r="AB10" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="AC10" s="10">
         <v>8</v>
       </c>
@@ -6703,7 +6984,9 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="17"/>
+      <c r="AB11" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="AC11" s="10">
         <v>8</v>
       </c>
@@ -6742,7 +7025,9 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="17"/>
+      <c r="AB12" s="17" t="s">
+        <v>180</v>
+      </c>
       <c r="AC12" s="10">
         <v>8</v>
       </c>
@@ -6781,7 +7066,9 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="17"/>
+      <c r="AB13" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="AC13" s="10">
         <v>8</v>
       </c>
@@ -6820,7 +7107,9 @@
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-      <c r="AB14" s="17"/>
+      <c r="AB14" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="AC14" s="10">
         <v>8</v>
       </c>
@@ -6859,7 +7148,9 @@
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-      <c r="AB15" s="17"/>
+      <c r="AB15" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="AC15" s="10">
         <v>8</v>
       </c>
@@ -6898,7 +7189,9 @@
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-      <c r="AB16" s="17"/>
+      <c r="AB16" s="17" t="s">
+        <v>184</v>
+      </c>
       <c r="AC16" s="10">
         <v>8</v>
       </c>
@@ -6937,7 +7230,9 @@
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
-      <c r="AB17" s="17"/>
+      <c r="AB17" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="AC17" s="10">
         <v>8</v>
       </c>
@@ -7483,37 +7778,37 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="39" t="s">
         <v>151</v>
       </c>
       <c r="L3" s="14"/>
@@ -7532,50 +7827,50 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="33" t="s">
+      <c r="AB3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="33" t="s">
+      <c r="AC3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="33" t="s">
+      <c r="AD3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33" t="s">
+      <c r="AE3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="33" t="s">
+      <c r="AF3" s="43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="45" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="39" t="s">
         <v>147</v>
       </c>
       <c r="L4" s="14"/>
@@ -7594,11 +7889,11 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
+      <c r="AE4" s="44"/>
+      <c r="AF4" s="44"/>
     </row>
     <row r="5" spans="1:32" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -7607,31 +7902,31 @@
       <c r="B5" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" s="43" t="s">
+      <c r="C5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="37" t="s">
         <v>100</v>
       </c>
       <c r="L5" s="10"/>
@@ -7649,7 +7944,7 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="37" t="s">
         <v>90</v>
       </c>
       <c r="AC5" s="10">
@@ -7688,7 +7983,7 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="37" t="s">
         <v>91</v>
       </c>
       <c r="AC6" s="10">
@@ -7727,7 +8022,7 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-      <c r="AB7" s="43" t="s">
+      <c r="AB7" s="37" t="s">
         <v>92</v>
       </c>
       <c r="AC7" s="10">
@@ -7766,7 +8061,7 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-      <c r="AB8" s="43" t="s">
+      <c r="AB8" s="37" t="s">
         <v>93</v>
       </c>
       <c r="AC8" s="10">
@@ -7805,7 +8100,7 @@
       <c r="X9" s="10"/>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
-      <c r="AB9" s="43" t="s">
+      <c r="AB9" s="37" t="s">
         <v>94</v>
       </c>
       <c r="AC9" s="10">
@@ -7844,7 +8139,7 @@
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
-      <c r="AB10" s="43" t="s">
+      <c r="AB10" s="37" t="s">
         <v>154</v>
       </c>
       <c r="AC10" s="10">
@@ -7883,7 +8178,7 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-      <c r="AB11" s="43" t="s">
+      <c r="AB11" s="37" t="s">
         <v>155</v>
       </c>
       <c r="AC11" s="10">
@@ -7922,7 +8217,7 @@
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
       <c r="Z12" s="10"/>
-      <c r="AB12" s="43" t="s">
+      <c r="AB12" s="37" t="s">
         <v>156</v>
       </c>
       <c r="AC12" s="10">
@@ -7961,7 +8256,7 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-      <c r="AB13" s="43" t="s">
+      <c r="AB13" s="37" t="s">
         <v>157</v>
       </c>
       <c r="AC13" s="10">
@@ -8102,470 +8397,631 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J21"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="32"/>
     <col min="5" max="5" width="9.140625" style="32"/>
+    <col min="11" max="11" width="9.140625" style="50"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="35">
         <v>2</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="35">
         <v>1</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="40">
+      <c r="G2" s="34">
         <v>4</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="40">
+      <c r="J2" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="K2" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="35">
         <v>2</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="35">
         <v>1</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="34">
         <v>4</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="40">
+      <c r="J3" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="K3" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="35">
         <v>2</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="35">
         <v>1</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="34">
         <v>4</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="J4" s="40">
+      <c r="J4" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+      <c r="K4" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="L4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="35">
         <v>2</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="35">
         <v>1</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="34">
         <v>5</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="K5" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="35">
         <v>2</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="35">
         <v>1</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="34">
         <v>5</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="34">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="K6" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="35">
         <v>2</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="35">
         <v>1</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="34">
         <v>4</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="34">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="K7" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="35">
         <v>2</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="35">
         <v>1</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="34">
         <v>2</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="34">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="K8" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="35">
         <v>4</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="35">
         <v>1</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="34">
         <v>2</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="J9" s="40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="J9" s="34">
+        <v>8</v>
+      </c>
+      <c r="K9" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="35">
         <v>4</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="41">
-        <v>8</v>
-      </c>
-      <c r="F10" s="40" t="s">
+      <c r="E10" s="35">
+        <v>8</v>
+      </c>
+      <c r="F10" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="34">
         <v>6</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="J10" s="34">
+        <v>8</v>
+      </c>
+      <c r="K10" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="35">
         <v>4</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="41">
-        <v>8</v>
-      </c>
-      <c r="F11" s="40" t="s">
+      <c r="E11" s="35">
+        <v>8</v>
+      </c>
+      <c r="F11" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="34">
         <v>6</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="J11" s="34">
+        <v>8</v>
+      </c>
+      <c r="K11" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="L11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="35">
         <v>4</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="41">
-        <v>8</v>
-      </c>
-      <c r="F12" s="40" t="s">
+      <c r="E12" s="35">
+        <v>8</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="34">
         <v>6</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="J12" s="40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="J12" s="34">
+        <v>8</v>
+      </c>
+      <c r="K12" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="35">
         <v>4</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="41">
-        <v>8</v>
-      </c>
-      <c r="F13" s="40" t="s">
+      <c r="E13" s="35">
+        <v>8</v>
+      </c>
+      <c r="F13" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="I13" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" s="34">
+        <v>3</v>
+      </c>
+      <c r="K13" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="L13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="35">
         <v>5</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="41">
-        <v>8</v>
-      </c>
-      <c r="F14" s="40" t="s">
+      <c r="E14" s="35">
+        <v>8</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="I14" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="J14" s="34">
+        <v>3</v>
+      </c>
+      <c r="K14" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="35">
         <v>5</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="35">
         <v>4</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="40" t="s">
+      <c r="I15" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" s="34">
+        <v>3</v>
+      </c>
+      <c r="K15" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="L15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="35">
         <v>5</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="35">
         <v>4</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+      <c r="I16" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="J16" s="34">
+        <v>3</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="L16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="35">
         <v>1</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="35">
         <v>4</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="I17" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="35">
         <v>1</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="35">
         <v>4</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="I18" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="35">
         <v>1</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="35">
         <v>4</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="I19" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="J19" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="35">
         <v>1</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="35">
         <v>4</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="34">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="40" t="s">
+      <c r="I20" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="J20" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="35">
         <v>4</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" s="34">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>